<commit_message>
added report and solve the multiple dept bug
</commit_message>
<xml_diff>
--- a/uploads/IS_training_format.xlsx
+++ b/uploads/IS_training_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bibun\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65EDAB9A-8833-45F8-973D-ABCC5BC5C9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC9BBE1B-35F2-4CAF-ABEA-F082938D674F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{76C125FD-4D31-49C0-86E3-7F8DC618CE13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{67DEE020-B61D-4CC6-AAB6-20E46BE7BA9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,54 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">S. No </t>
+    <t>sl no.</t>
   </si>
   <si>
-    <t xml:space="preserve">Name of Program </t>
+    <t>training name</t>
   </si>
   <si>
-    <t>Type</t>
+    <t xml:space="preserve">description </t>
   </si>
   <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>Nos/Year</t>
-  </si>
-  <si>
-    <t>Scheduled Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faculty Type </t>
-  </si>
-  <si>
-    <t>Faculty \FPR Dept</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Part. Department</t>
-  </si>
-  <si>
-    <t>OISD Mapping</t>
-  </si>
-  <si>
-    <t>OISD Mapping 100% Coverage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remarks </t>
-  </si>
-  <si>
-    <t>Lowest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highest </t>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -105,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -113,69 +77,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,102 +396,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC9FBCB-DD02-4AC8-A838-B585CA4EC10D}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F0E391-8F40-40EF-ABC4-FAEED80FBEDB}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>